<commit_message>
making float test better; improving language on website
</commit_message>
<xml_diff>
--- a/src/test/resources/data_integration_tests/test_malformed_parse_float.xlsx
+++ b/src/test/resources/data_integration_tests/test_malformed_parse_float.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>Unit</t>
   </si>
@@ -50,12 +50,18 @@
   <si>
     <t xml:space="preserve">1F </t>
   </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>02588.000F</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +93,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,12 +115,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -110,11 +144,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -449,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A226" sqref="A226"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -462,7 +500,7 @@
     <col min="3" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +510,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>4812</v>
       </c>
@@ -483,8 +524,11 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>4812</v>
       </c>
@@ -495,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4812</v>
       </c>
@@ -506,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4812</v>
       </c>
@@ -517,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4812</v>
       </c>
@@ -528,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>4812</v>
       </c>
@@ -539,7 +583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>4812</v>
       </c>
@@ -550,7 +594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>4812</v>
       </c>
@@ -561,7 +605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>4812</v>
       </c>
@@ -572,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>4812</v>
       </c>
@@ -583,7 +627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>4812</v>
       </c>
@@ -594,7 +638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>4812</v>
       </c>
@@ -605,7 +649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>4812</v>
       </c>
@@ -616,7 +660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>4812</v>
       </c>
@@ -627,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>4812</v>
       </c>

</xml_diff>